<commit_message>
Angefangene Stücklisten für Drohne und Anhänger
</commit_message>
<xml_diff>
--- a/Meilenstein 4/Dokumente/Stückliste_Schienensystem.xlsx
+++ b/Meilenstein 4/Dokumente/Stückliste_Schienensystem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Methodisches Konstruieren\Übungen\git repo\MKon\Meilenstein 4\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B5A2A-DC7B-412B-AB51-CBC404A689BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A6A4AE-5F0C-4441-B4F0-7466B3588AE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8629A93B-4D8D-4644-A0F5-A6E2E52E581F}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8629A93B-4D8D-4644-A0F5-A6E2E52E581F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>